<commit_message>
New models and measurements
</commit_message>
<xml_diff>
--- a/Models to measure/Results/Filtered loss plots/Amount of plateaus.xlsx
+++ b/Models to measure/Results/Filtered loss plots/Amount of plateaus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20182672\Documents\GitHub\Final_Project\Models to measure\Results\Filtered loss plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF00A95B-AFB5-4C61-8D60-94001A8E4D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DCBB41-ED45-4E4D-87E9-8D12C038977B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21108" yWindow="3408" windowWidth="2388" windowHeight="564" xr2:uid="{98A813E1-F41E-4DF4-9B2F-04D1C5B250A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98A813E1-F41E-4DF4-9B2F-04D1C5B250A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,23 +403,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED336A5-05FC-4E6D-9199-11645426FC6F}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
+      <selection activeCell="F293" sqref="F293"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -439,7 +439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -479,7 +479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -519,7 +519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -539,7 +539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -559,9 +559,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -579,9 +579,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -639,7 +639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -659,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -679,7 +679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -699,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -719,7 +719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -739,7 +739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -759,7 +759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -799,7 +799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -819,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -839,7 +839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -879,9 +879,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -899,9 +899,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -919,7 +919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -959,7 +959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -979,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -999,7 +999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1139,9 +1139,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1159,9 +1159,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1179,9 +1179,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1199,7 +1199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1419,9 +1419,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1439,9 +1439,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1459,7 +1459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0</v>
       </c>
@@ -1719,9 +1719,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -1739,9 +1739,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -1759,7 +1759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0</v>
       </c>
@@ -2059,9 +2059,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2079,9 +2079,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2099,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0</v>
       </c>
@@ -2359,9 +2359,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2379,9 +2379,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2399,7 +2399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1</v>
       </c>
@@ -2537,6 +2537,3706 @@
       </c>
       <c r="F106">
         <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>25</v>
+      </c>
+      <c r="D107">
+        <v>10</v>
+      </c>
+      <c r="E107">
+        <v>6</v>
+      </c>
+      <c r="F107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>1</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>25</v>
+      </c>
+      <c r="D108">
+        <v>10</v>
+      </c>
+      <c r="E108">
+        <v>6</v>
+      </c>
+      <c r="F108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>25</v>
+      </c>
+      <c r="D109">
+        <v>20</v>
+      </c>
+      <c r="E109">
+        <v>7</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>25</v>
+      </c>
+      <c r="D110">
+        <v>20</v>
+      </c>
+      <c r="E110">
+        <v>7</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>25</v>
+      </c>
+      <c r="D111">
+        <v>20</v>
+      </c>
+      <c r="E111">
+        <v>7</v>
+      </c>
+      <c r="F111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1</v>
+      </c>
+      <c r="B112">
+        <v>4</v>
+      </c>
+      <c r="C112">
+        <v>25</v>
+      </c>
+      <c r="D112">
+        <v>20</v>
+      </c>
+      <c r="E112">
+        <v>7</v>
+      </c>
+      <c r="F112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>25</v>
+      </c>
+      <c r="D113">
+        <v>10</v>
+      </c>
+      <c r="E113">
+        <v>6</v>
+      </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>25</v>
+      </c>
+      <c r="D114">
+        <v>10</v>
+      </c>
+      <c r="E114">
+        <v>6</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115">
+        <v>4</v>
+      </c>
+      <c r="C115">
+        <v>50</v>
+      </c>
+      <c r="D115">
+        <v>20</v>
+      </c>
+      <c r="E115">
+        <v>7</v>
+      </c>
+      <c r="F115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>50</v>
+      </c>
+      <c r="D116">
+        <v>10</v>
+      </c>
+      <c r="E116">
+        <v>6</v>
+      </c>
+      <c r="F116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>50</v>
+      </c>
+      <c r="D117">
+        <v>10</v>
+      </c>
+      <c r="E117">
+        <v>6</v>
+      </c>
+      <c r="F117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118">
+        <v>3</v>
+      </c>
+      <c r="C118">
+        <v>50</v>
+      </c>
+      <c r="D118">
+        <v>20</v>
+      </c>
+      <c r="E118">
+        <v>7</v>
+      </c>
+      <c r="F118">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="C119">
+        <v>50</v>
+      </c>
+      <c r="D119">
+        <v>20</v>
+      </c>
+      <c r="E119">
+        <v>7</v>
+      </c>
+      <c r="F119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>1</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>50</v>
+      </c>
+      <c r="D120">
+        <v>10</v>
+      </c>
+      <c r="E120">
+        <v>6</v>
+      </c>
+      <c r="F120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1</v>
+      </c>
+      <c r="B121">
+        <v>8</v>
+      </c>
+      <c r="C121">
+        <v>50</v>
+      </c>
+      <c r="D121">
+        <v>10</v>
+      </c>
+      <c r="E121">
+        <v>6</v>
+      </c>
+      <c r="F121">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>50</v>
+      </c>
+      <c r="D122">
+        <v>20</v>
+      </c>
+      <c r="E122">
+        <v>7</v>
+      </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>75</v>
+      </c>
+      <c r="D123">
+        <v>10</v>
+      </c>
+      <c r="E123">
+        <v>6</v>
+      </c>
+      <c r="F123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>75</v>
+      </c>
+      <c r="D124">
+        <v>10</v>
+      </c>
+      <c r="E124">
+        <v>6</v>
+      </c>
+      <c r="F124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>1</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>75</v>
+      </c>
+      <c r="D125">
+        <v>20</v>
+      </c>
+      <c r="E125">
+        <v>7</v>
+      </c>
+      <c r="F125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>7</v>
+      </c>
+      <c r="C126">
+        <v>75</v>
+      </c>
+      <c r="D126">
+        <v>20</v>
+      </c>
+      <c r="E126">
+        <v>7</v>
+      </c>
+      <c r="F126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>1</v>
+      </c>
+      <c r="B127">
+        <v>9</v>
+      </c>
+      <c r="C127">
+        <v>75</v>
+      </c>
+      <c r="D127">
+        <v>10</v>
+      </c>
+      <c r="E127">
+        <v>6</v>
+      </c>
+      <c r="F127">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>1</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>75</v>
+      </c>
+      <c r="D128">
+        <v>10</v>
+      </c>
+      <c r="E128">
+        <v>6</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>1</v>
+      </c>
+      <c r="B129">
+        <v>4</v>
+      </c>
+      <c r="C129">
+        <v>75</v>
+      </c>
+      <c r="D129">
+        <v>20</v>
+      </c>
+      <c r="E129">
+        <v>7</v>
+      </c>
+      <c r="F129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>1</v>
+      </c>
+      <c r="B130">
+        <v>3</v>
+      </c>
+      <c r="C130">
+        <v>75</v>
+      </c>
+      <c r="D130">
+        <v>20</v>
+      </c>
+      <c r="E130">
+        <v>7</v>
+      </c>
+      <c r="F130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>4</v>
+      </c>
+      <c r="C131">
+        <v>100</v>
+      </c>
+      <c r="D131">
+        <v>20</v>
+      </c>
+      <c r="E131">
+        <v>7</v>
+      </c>
+      <c r="F131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>1</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>100</v>
+      </c>
+      <c r="D132">
+        <v>20</v>
+      </c>
+      <c r="E132">
+        <v>7</v>
+      </c>
+      <c r="F132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>1</v>
+      </c>
+      <c r="B133">
+        <v>6</v>
+      </c>
+      <c r="C133">
+        <v>100</v>
+      </c>
+      <c r="D133">
+        <v>20</v>
+      </c>
+      <c r="E133">
+        <v>7</v>
+      </c>
+      <c r="F133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>1</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>100</v>
+      </c>
+      <c r="D134">
+        <v>10</v>
+      </c>
+      <c r="E134">
+        <v>6</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>100</v>
+      </c>
+      <c r="D135">
+        <v>10</v>
+      </c>
+      <c r="E135">
+        <v>6</v>
+      </c>
+      <c r="F135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>1</v>
+      </c>
+      <c r="B136">
+        <v>4</v>
+      </c>
+      <c r="C136">
+        <v>100</v>
+      </c>
+      <c r="D136">
+        <v>20</v>
+      </c>
+      <c r="E136">
+        <v>7</v>
+      </c>
+      <c r="F136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>1</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>100</v>
+      </c>
+      <c r="D137">
+        <v>10</v>
+      </c>
+      <c r="E137">
+        <v>6</v>
+      </c>
+      <c r="F137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>1</v>
+      </c>
+      <c r="B138">
+        <v>2</v>
+      </c>
+      <c r="C138">
+        <v>100</v>
+      </c>
+      <c r="D138">
+        <v>10</v>
+      </c>
+      <c r="E138">
+        <v>6</v>
+      </c>
+      <c r="F138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>125</v>
+      </c>
+      <c r="D139">
+        <v>10</v>
+      </c>
+      <c r="E139">
+        <v>6</v>
+      </c>
+      <c r="F139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>1</v>
+      </c>
+      <c r="B140">
+        <v>7</v>
+      </c>
+      <c r="C140">
+        <v>125</v>
+      </c>
+      <c r="D140">
+        <v>10</v>
+      </c>
+      <c r="E140">
+        <v>6</v>
+      </c>
+      <c r="F140">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>1</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>125</v>
+      </c>
+      <c r="D141">
+        <v>10</v>
+      </c>
+      <c r="E141">
+        <v>6</v>
+      </c>
+      <c r="F141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>1</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>125</v>
+      </c>
+      <c r="D142">
+        <v>10</v>
+      </c>
+      <c r="E142">
+        <v>6</v>
+      </c>
+      <c r="F142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1</v>
+      </c>
+      <c r="B143">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>125</v>
+      </c>
+      <c r="D143">
+        <v>20</v>
+      </c>
+      <c r="E143">
+        <v>7</v>
+      </c>
+      <c r="F143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>1</v>
+      </c>
+      <c r="B144">
+        <v>3</v>
+      </c>
+      <c r="C144">
+        <v>125</v>
+      </c>
+      <c r="D144">
+        <v>20</v>
+      </c>
+      <c r="E144">
+        <v>7</v>
+      </c>
+      <c r="F144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>1</v>
+      </c>
+      <c r="B145">
+        <v>7</v>
+      </c>
+      <c r="C145">
+        <v>125</v>
+      </c>
+      <c r="D145">
+        <v>20</v>
+      </c>
+      <c r="E145">
+        <v>7</v>
+      </c>
+      <c r="F145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>125</v>
+      </c>
+      <c r="D146">
+        <v>20</v>
+      </c>
+      <c r="E146">
+        <v>7</v>
+      </c>
+      <c r="F146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>1</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>150</v>
+      </c>
+      <c r="D147">
+        <v>10</v>
+      </c>
+      <c r="E147">
+        <v>6</v>
+      </c>
+      <c r="F147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+      <c r="C148">
+        <v>150</v>
+      </c>
+      <c r="D148">
+        <v>20</v>
+      </c>
+      <c r="E148">
+        <v>7</v>
+      </c>
+      <c r="F148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>150</v>
+      </c>
+      <c r="D149">
+        <v>10</v>
+      </c>
+      <c r="E149">
+        <v>6</v>
+      </c>
+      <c r="F149">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>1</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>150</v>
+      </c>
+      <c r="D150">
+        <v>10</v>
+      </c>
+      <c r="E150">
+        <v>6</v>
+      </c>
+      <c r="F150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>4</v>
+      </c>
+      <c r="C151">
+        <v>150</v>
+      </c>
+      <c r="D151">
+        <v>20</v>
+      </c>
+      <c r="E151">
+        <v>7</v>
+      </c>
+      <c r="F151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>1</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>150</v>
+      </c>
+      <c r="D152">
+        <v>10</v>
+      </c>
+      <c r="E152">
+        <v>6</v>
+      </c>
+      <c r="F152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>1</v>
+      </c>
+      <c r="B153">
+        <v>3</v>
+      </c>
+      <c r="C153">
+        <v>150</v>
+      </c>
+      <c r="D153">
+        <v>20</v>
+      </c>
+      <c r="E153">
+        <v>7</v>
+      </c>
+      <c r="F153">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>150</v>
+      </c>
+      <c r="D154">
+        <v>20</v>
+      </c>
+      <c r="E154">
+        <v>7</v>
+      </c>
+      <c r="F154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>175</v>
+      </c>
+      <c r="D155">
+        <v>10</v>
+      </c>
+      <c r="E155">
+        <v>6</v>
+      </c>
+      <c r="F155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>1</v>
+      </c>
+      <c r="B156">
+        <v>4</v>
+      </c>
+      <c r="C156">
+        <v>175</v>
+      </c>
+      <c r="D156">
+        <v>20</v>
+      </c>
+      <c r="E156">
+        <v>7</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>175</v>
+      </c>
+      <c r="D157">
+        <v>10</v>
+      </c>
+      <c r="E157">
+        <v>6</v>
+      </c>
+      <c r="F157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>1</v>
+      </c>
+      <c r="B158">
+        <v>2</v>
+      </c>
+      <c r="C158">
+        <v>175</v>
+      </c>
+      <c r="D158">
+        <v>10</v>
+      </c>
+      <c r="E158">
+        <v>6</v>
+      </c>
+      <c r="F158">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>1</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>175</v>
+      </c>
+      <c r="D159">
+        <v>10</v>
+      </c>
+      <c r="E159">
+        <v>5</v>
+      </c>
+      <c r="F159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>175</v>
+      </c>
+      <c r="D160">
+        <v>10</v>
+      </c>
+      <c r="E160">
+        <v>6</v>
+      </c>
+      <c r="F160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>175</v>
+      </c>
+      <c r="D161">
+        <v>20</v>
+      </c>
+      <c r="E161">
+        <v>7</v>
+      </c>
+      <c r="F161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>175</v>
+      </c>
+      <c r="D162">
+        <v>10</v>
+      </c>
+      <c r="E162">
+        <v>5</v>
+      </c>
+      <c r="F162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>1</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+      <c r="C163">
+        <v>175</v>
+      </c>
+      <c r="D163">
+        <v>10</v>
+      </c>
+      <c r="E163">
+        <v>5</v>
+      </c>
+      <c r="F163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>1</v>
+      </c>
+      <c r="B164">
+        <v>4</v>
+      </c>
+      <c r="C164">
+        <v>175</v>
+      </c>
+      <c r="D164">
+        <v>20</v>
+      </c>
+      <c r="E164">
+        <v>7</v>
+      </c>
+      <c r="F164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>1</v>
+      </c>
+      <c r="B165">
+        <v>6</v>
+      </c>
+      <c r="C165">
+        <v>175</v>
+      </c>
+      <c r="D165">
+        <v>20</v>
+      </c>
+      <c r="E165">
+        <v>7</v>
+      </c>
+      <c r="F165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>1</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>175</v>
+      </c>
+      <c r="D166">
+        <v>10</v>
+      </c>
+      <c r="E166">
+        <v>5</v>
+      </c>
+      <c r="F166">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>1</v>
+      </c>
+      <c r="B167">
+        <v>3</v>
+      </c>
+      <c r="C167">
+        <v>175</v>
+      </c>
+      <c r="D167">
+        <v>50</v>
+      </c>
+      <c r="E167">
+        <v>8</v>
+      </c>
+      <c r="F167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>1</v>
+      </c>
+      <c r="B168">
+        <v>6</v>
+      </c>
+      <c r="C168">
+        <v>175</v>
+      </c>
+      <c r="D168">
+        <v>50</v>
+      </c>
+      <c r="E168">
+        <v>8</v>
+      </c>
+      <c r="F168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>1</v>
+      </c>
+      <c r="B169">
+        <v>3</v>
+      </c>
+      <c r="C169">
+        <v>175</v>
+      </c>
+      <c r="D169">
+        <v>100</v>
+      </c>
+      <c r="E169">
+        <v>10</v>
+      </c>
+      <c r="F169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>1</v>
+      </c>
+      <c r="B170">
+        <v>5</v>
+      </c>
+      <c r="C170">
+        <v>175</v>
+      </c>
+      <c r="D170">
+        <v>50</v>
+      </c>
+      <c r="E170">
+        <v>9</v>
+      </c>
+      <c r="F170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1</v>
+      </c>
+      <c r="B171">
+        <v>6</v>
+      </c>
+      <c r="C171">
+        <v>175</v>
+      </c>
+      <c r="D171">
+        <v>100</v>
+      </c>
+      <c r="E171">
+        <v>10</v>
+      </c>
+      <c r="F171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>1</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+      <c r="C172">
+        <v>175</v>
+      </c>
+      <c r="D172">
+        <v>50</v>
+      </c>
+      <c r="E172">
+        <v>9</v>
+      </c>
+      <c r="F172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>1</v>
+      </c>
+      <c r="B173">
+        <v>3</v>
+      </c>
+      <c r="C173">
+        <v>175</v>
+      </c>
+      <c r="D173">
+        <v>50</v>
+      </c>
+      <c r="E173">
+        <v>8</v>
+      </c>
+      <c r="F173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>1</v>
+      </c>
+      <c r="B174">
+        <v>2</v>
+      </c>
+      <c r="C174">
+        <v>175</v>
+      </c>
+      <c r="D174">
+        <v>50</v>
+      </c>
+      <c r="E174">
+        <v>8</v>
+      </c>
+      <c r="F174">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>1</v>
+      </c>
+      <c r="B175">
+        <v>8</v>
+      </c>
+      <c r="C175">
+        <v>175</v>
+      </c>
+      <c r="D175">
+        <v>100</v>
+      </c>
+      <c r="E175">
+        <v>10</v>
+      </c>
+      <c r="F175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>1</v>
+      </c>
+      <c r="B176">
+        <v>6</v>
+      </c>
+      <c r="C176">
+        <v>175</v>
+      </c>
+      <c r="D176">
+        <v>50</v>
+      </c>
+      <c r="E176">
+        <v>9</v>
+      </c>
+      <c r="F176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>1</v>
+      </c>
+      <c r="B177">
+        <v>2</v>
+      </c>
+      <c r="C177">
+        <v>175</v>
+      </c>
+      <c r="D177">
+        <v>100</v>
+      </c>
+      <c r="E177">
+        <v>10</v>
+      </c>
+      <c r="F177">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>1</v>
+      </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <v>200</v>
+      </c>
+      <c r="D178">
+        <v>10</v>
+      </c>
+      <c r="E178">
+        <v>5</v>
+      </c>
+      <c r="F178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>1</v>
+      </c>
+      <c r="B179">
+        <v>6</v>
+      </c>
+      <c r="C179">
+        <v>200</v>
+      </c>
+      <c r="D179">
+        <v>20</v>
+      </c>
+      <c r="E179">
+        <v>7</v>
+      </c>
+      <c r="F179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>1</v>
+      </c>
+      <c r="B180">
+        <v>2</v>
+      </c>
+      <c r="C180">
+        <v>200</v>
+      </c>
+      <c r="D180">
+        <v>10</v>
+      </c>
+      <c r="E180">
+        <v>6</v>
+      </c>
+      <c r="F180">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>1</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>200</v>
+      </c>
+      <c r="D181">
+        <v>20</v>
+      </c>
+      <c r="E181">
+        <v>7</v>
+      </c>
+      <c r="F181">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>1</v>
+      </c>
+      <c r="B182">
+        <v>0</v>
+      </c>
+      <c r="C182">
+        <v>200</v>
+      </c>
+      <c r="D182">
+        <v>10</v>
+      </c>
+      <c r="E182">
+        <v>5</v>
+      </c>
+      <c r="F182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>1</v>
+      </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <v>200</v>
+      </c>
+      <c r="D183">
+        <v>10</v>
+      </c>
+      <c r="E183">
+        <v>6</v>
+      </c>
+      <c r="F183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>1</v>
+      </c>
+      <c r="B184">
+        <v>5</v>
+      </c>
+      <c r="C184">
+        <v>200</v>
+      </c>
+      <c r="D184">
+        <v>20</v>
+      </c>
+      <c r="E184">
+        <v>7</v>
+      </c>
+      <c r="F184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>1</v>
+      </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <v>200</v>
+      </c>
+      <c r="D185">
+        <v>10</v>
+      </c>
+      <c r="E185">
+        <v>6</v>
+      </c>
+      <c r="F185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>1</v>
+      </c>
+      <c r="B186">
+        <v>0</v>
+      </c>
+      <c r="C186">
+        <v>200</v>
+      </c>
+      <c r="D186">
+        <v>10</v>
+      </c>
+      <c r="E186">
+        <v>5</v>
+      </c>
+      <c r="F186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>1</v>
+      </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
+      <c r="C187">
+        <v>200</v>
+      </c>
+      <c r="D187">
+        <v>10</v>
+      </c>
+      <c r="E187">
+        <v>5</v>
+      </c>
+      <c r="F187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>1</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188">
+        <v>200</v>
+      </c>
+      <c r="D188">
+        <v>10</v>
+      </c>
+      <c r="E188">
+        <v>6</v>
+      </c>
+      <c r="F188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>1</v>
+      </c>
+      <c r="B189">
+        <v>12</v>
+      </c>
+      <c r="C189">
+        <v>200</v>
+      </c>
+      <c r="D189">
+        <v>20</v>
+      </c>
+      <c r="E189">
+        <v>7</v>
+      </c>
+      <c r="F189">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>1</v>
+      </c>
+      <c r="B190">
+        <v>6</v>
+      </c>
+      <c r="C190">
+        <v>200</v>
+      </c>
+      <c r="D190">
+        <v>100</v>
+      </c>
+      <c r="E190">
+        <v>10</v>
+      </c>
+      <c r="F190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>1</v>
+      </c>
+      <c r="B191">
+        <v>6</v>
+      </c>
+      <c r="C191">
+        <v>200</v>
+      </c>
+      <c r="D191">
+        <v>100</v>
+      </c>
+      <c r="E191">
+        <v>10</v>
+      </c>
+      <c r="F191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>1</v>
+      </c>
+      <c r="B192">
+        <v>9</v>
+      </c>
+      <c r="C192">
+        <v>200</v>
+      </c>
+      <c r="D192">
+        <v>50</v>
+      </c>
+      <c r="E192">
+        <v>9</v>
+      </c>
+      <c r="F192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>1</v>
+      </c>
+      <c r="B193">
+        <v>2</v>
+      </c>
+      <c r="C193">
+        <v>200</v>
+      </c>
+      <c r="D193">
+        <v>50</v>
+      </c>
+      <c r="E193">
+        <v>8</v>
+      </c>
+      <c r="F193">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>1</v>
+      </c>
+      <c r="B194">
+        <v>3</v>
+      </c>
+      <c r="C194">
+        <v>200</v>
+      </c>
+      <c r="D194">
+        <v>100</v>
+      </c>
+      <c r="E194">
+        <v>10</v>
+      </c>
+      <c r="F194">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>1</v>
+      </c>
+      <c r="B195">
+        <v>4</v>
+      </c>
+      <c r="C195">
+        <v>200</v>
+      </c>
+      <c r="D195">
+        <v>50</v>
+      </c>
+      <c r="E195">
+        <v>8</v>
+      </c>
+      <c r="F195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>1</v>
+      </c>
+      <c r="B196">
+        <v>1</v>
+      </c>
+      <c r="C196">
+        <v>200</v>
+      </c>
+      <c r="D196">
+        <v>50</v>
+      </c>
+      <c r="E196">
+        <v>8</v>
+      </c>
+      <c r="F196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>1</v>
+      </c>
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <v>200</v>
+      </c>
+      <c r="D197">
+        <v>50</v>
+      </c>
+      <c r="E197">
+        <v>8</v>
+      </c>
+      <c r="F197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>1</v>
+      </c>
+      <c r="B198">
+        <v>6</v>
+      </c>
+      <c r="C198">
+        <v>200</v>
+      </c>
+      <c r="D198">
+        <v>50</v>
+      </c>
+      <c r="E198">
+        <v>8</v>
+      </c>
+      <c r="F198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>1</v>
+      </c>
+      <c r="B199">
+        <v>4</v>
+      </c>
+      <c r="C199">
+        <v>200</v>
+      </c>
+      <c r="D199">
+        <v>100</v>
+      </c>
+      <c r="E199">
+        <v>10</v>
+      </c>
+      <c r="F199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>1</v>
+      </c>
+      <c r="B200">
+        <v>8</v>
+      </c>
+      <c r="C200">
+        <v>200</v>
+      </c>
+      <c r="D200">
+        <v>50</v>
+      </c>
+      <c r="E200">
+        <v>9</v>
+      </c>
+      <c r="F200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>1</v>
+      </c>
+      <c r="B201">
+        <v>0</v>
+      </c>
+      <c r="C201">
+        <v>225</v>
+      </c>
+      <c r="D201">
+        <v>10</v>
+      </c>
+      <c r="E201">
+        <v>5</v>
+      </c>
+      <c r="F201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>0</v>
+      </c>
+      <c r="B202">
+        <v>0</v>
+      </c>
+      <c r="C202">
+        <v>225</v>
+      </c>
+      <c r="D202">
+        <v>10</v>
+      </c>
+      <c r="E202">
+        <v>5</v>
+      </c>
+      <c r="F202">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>1</v>
+      </c>
+      <c r="B203">
+        <v>0</v>
+      </c>
+      <c r="C203">
+        <v>225</v>
+      </c>
+      <c r="D203">
+        <v>10</v>
+      </c>
+      <c r="E203">
+        <v>5</v>
+      </c>
+      <c r="F203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>1</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>225</v>
+      </c>
+      <c r="D204">
+        <v>10</v>
+      </c>
+      <c r="E204">
+        <v>6</v>
+      </c>
+      <c r="F204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>1</v>
+      </c>
+      <c r="B205">
+        <v>3</v>
+      </c>
+      <c r="C205">
+        <v>225</v>
+      </c>
+      <c r="D205">
+        <v>20</v>
+      </c>
+      <c r="E205">
+        <v>7</v>
+      </c>
+      <c r="F205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>1</v>
+      </c>
+      <c r="B206">
+        <v>0</v>
+      </c>
+      <c r="C206">
+        <v>225</v>
+      </c>
+      <c r="D206">
+        <v>10</v>
+      </c>
+      <c r="E206">
+        <v>6</v>
+      </c>
+      <c r="F206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>1</v>
+      </c>
+      <c r="B207">
+        <v>0</v>
+      </c>
+      <c r="C207">
+        <v>225</v>
+      </c>
+      <c r="D207">
+        <v>10</v>
+      </c>
+      <c r="E207">
+        <v>6</v>
+      </c>
+      <c r="F207">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>1</v>
+      </c>
+      <c r="B208">
+        <v>8</v>
+      </c>
+      <c r="C208">
+        <v>225</v>
+      </c>
+      <c r="D208">
+        <v>20</v>
+      </c>
+      <c r="E208">
+        <v>7</v>
+      </c>
+      <c r="F208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>1</v>
+      </c>
+      <c r="B209">
+        <v>0</v>
+      </c>
+      <c r="C209">
+        <v>225</v>
+      </c>
+      <c r="D209">
+        <v>20</v>
+      </c>
+      <c r="E209">
+        <v>7</v>
+      </c>
+      <c r="F209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>1</v>
+      </c>
+      <c r="B210">
+        <v>6</v>
+      </c>
+      <c r="C210">
+        <v>225</v>
+      </c>
+      <c r="D210">
+        <v>20</v>
+      </c>
+      <c r="E210">
+        <v>7</v>
+      </c>
+      <c r="F210">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>1</v>
+      </c>
+      <c r="B211">
+        <v>0</v>
+      </c>
+      <c r="C211">
+        <v>225</v>
+      </c>
+      <c r="D211">
+        <v>10</v>
+      </c>
+      <c r="E211">
+        <v>6</v>
+      </c>
+      <c r="F211">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>1</v>
+      </c>
+      <c r="B212">
+        <v>0</v>
+      </c>
+      <c r="C212">
+        <v>225</v>
+      </c>
+      <c r="D212">
+        <v>10</v>
+      </c>
+      <c r="E212">
+        <v>5</v>
+      </c>
+      <c r="F212">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>1</v>
+      </c>
+      <c r="B213">
+        <v>3</v>
+      </c>
+      <c r="C213">
+        <v>225</v>
+      </c>
+      <c r="D213">
+        <v>50</v>
+      </c>
+      <c r="E213">
+        <v>8</v>
+      </c>
+      <c r="F213">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>1</v>
+      </c>
+      <c r="B214">
+        <v>3</v>
+      </c>
+      <c r="C214">
+        <v>225</v>
+      </c>
+      <c r="D214">
+        <v>100</v>
+      </c>
+      <c r="E214">
+        <v>10</v>
+      </c>
+      <c r="F214">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>1</v>
+      </c>
+      <c r="B215">
+        <v>6</v>
+      </c>
+      <c r="C215">
+        <v>225</v>
+      </c>
+      <c r="D215">
+        <v>50</v>
+      </c>
+      <c r="E215">
+        <v>9</v>
+      </c>
+      <c r="F215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>1</v>
+      </c>
+      <c r="B216">
+        <v>4</v>
+      </c>
+      <c r="C216">
+        <v>225</v>
+      </c>
+      <c r="D216">
+        <v>50</v>
+      </c>
+      <c r="E216">
+        <v>8</v>
+      </c>
+      <c r="F216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>1</v>
+      </c>
+      <c r="B217">
+        <v>3</v>
+      </c>
+      <c r="C217">
+        <v>225</v>
+      </c>
+      <c r="D217">
+        <v>50</v>
+      </c>
+      <c r="E217">
+        <v>8</v>
+      </c>
+      <c r="F217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>1</v>
+      </c>
+      <c r="B218">
+        <v>9</v>
+      </c>
+      <c r="C218">
+        <v>225</v>
+      </c>
+      <c r="D218">
+        <v>100</v>
+      </c>
+      <c r="E218">
+        <v>10</v>
+      </c>
+      <c r="F218">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>1</v>
+      </c>
+      <c r="B219">
+        <v>0</v>
+      </c>
+      <c r="C219">
+        <v>225</v>
+      </c>
+      <c r="D219">
+        <v>50</v>
+      </c>
+      <c r="E219">
+        <v>9</v>
+      </c>
+      <c r="F219">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>1</v>
+      </c>
+      <c r="B220">
+        <v>1</v>
+      </c>
+      <c r="C220">
+        <v>225</v>
+      </c>
+      <c r="D220">
+        <v>50</v>
+      </c>
+      <c r="E220">
+        <v>8</v>
+      </c>
+      <c r="F220">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>1</v>
+      </c>
+      <c r="B221">
+        <v>5</v>
+      </c>
+      <c r="C221">
+        <v>225</v>
+      </c>
+      <c r="D221">
+        <v>50</v>
+      </c>
+      <c r="E221">
+        <v>9</v>
+      </c>
+      <c r="F221">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>1</v>
+      </c>
+      <c r="B222">
+        <v>1</v>
+      </c>
+      <c r="C222">
+        <v>225</v>
+      </c>
+      <c r="D222">
+        <v>100</v>
+      </c>
+      <c r="E222">
+        <v>10</v>
+      </c>
+      <c r="F222">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>1</v>
+      </c>
+      <c r="B223">
+        <v>6</v>
+      </c>
+      <c r="C223">
+        <v>225</v>
+      </c>
+      <c r="D223">
+        <v>100</v>
+      </c>
+      <c r="E223">
+        <v>10</v>
+      </c>
+      <c r="F223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>1</v>
+      </c>
+      <c r="B224">
+        <v>0</v>
+      </c>
+      <c r="C224">
+        <v>250</v>
+      </c>
+      <c r="D224">
+        <v>10</v>
+      </c>
+      <c r="E224">
+        <v>6</v>
+      </c>
+      <c r="F224">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>1</v>
+      </c>
+      <c r="B225">
+        <v>5</v>
+      </c>
+      <c r="C225">
+        <v>250</v>
+      </c>
+      <c r="D225">
+        <v>20</v>
+      </c>
+      <c r="E225">
+        <v>7</v>
+      </c>
+      <c r="F225">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>1</v>
+      </c>
+      <c r="B226">
+        <v>4</v>
+      </c>
+      <c r="C226">
+        <v>250</v>
+      </c>
+      <c r="D226">
+        <v>20</v>
+      </c>
+      <c r="E226">
+        <v>7</v>
+      </c>
+      <c r="F226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>1</v>
+      </c>
+      <c r="B227">
+        <v>0</v>
+      </c>
+      <c r="C227">
+        <v>250</v>
+      </c>
+      <c r="D227">
+        <v>10</v>
+      </c>
+      <c r="E227">
+        <v>6</v>
+      </c>
+      <c r="F227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>1</v>
+      </c>
+      <c r="B228">
+        <v>0</v>
+      </c>
+      <c r="C228">
+        <v>250</v>
+      </c>
+      <c r="D228">
+        <v>20</v>
+      </c>
+      <c r="E228">
+        <v>7</v>
+      </c>
+      <c r="F228">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>1</v>
+      </c>
+      <c r="B229">
+        <v>0</v>
+      </c>
+      <c r="C229">
+        <v>250</v>
+      </c>
+      <c r="D229">
+        <v>10</v>
+      </c>
+      <c r="E229">
+        <v>6</v>
+      </c>
+      <c r="F229">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>1</v>
+      </c>
+      <c r="B230">
+        <v>0</v>
+      </c>
+      <c r="C230">
+        <v>250</v>
+      </c>
+      <c r="D230">
+        <v>10</v>
+      </c>
+      <c r="E230">
+        <v>6</v>
+      </c>
+      <c r="F230">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>1</v>
+      </c>
+      <c r="B231">
+        <v>0</v>
+      </c>
+      <c r="C231">
+        <v>250</v>
+      </c>
+      <c r="D231">
+        <v>10</v>
+      </c>
+      <c r="E231">
+        <v>5</v>
+      </c>
+      <c r="F231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>1</v>
+      </c>
+      <c r="B232">
+        <v>7</v>
+      </c>
+      <c r="C232">
+        <v>250</v>
+      </c>
+      <c r="D232">
+        <v>20</v>
+      </c>
+      <c r="E232">
+        <v>7</v>
+      </c>
+      <c r="F232">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>1</v>
+      </c>
+      <c r="B233">
+        <v>0</v>
+      </c>
+      <c r="C233">
+        <v>250</v>
+      </c>
+      <c r="D233">
+        <v>10</v>
+      </c>
+      <c r="E233">
+        <v>5</v>
+      </c>
+      <c r="F233">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>1</v>
+      </c>
+      <c r="B234">
+        <v>0</v>
+      </c>
+      <c r="C234">
+        <v>250</v>
+      </c>
+      <c r="D234">
+        <v>10</v>
+      </c>
+      <c r="E234">
+        <v>6</v>
+      </c>
+      <c r="F234">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>1</v>
+      </c>
+      <c r="B235">
+        <v>0</v>
+      </c>
+      <c r="C235">
+        <v>250</v>
+      </c>
+      <c r="D235">
+        <v>10</v>
+      </c>
+      <c r="E235">
+        <v>5</v>
+      </c>
+      <c r="F235">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>1</v>
+      </c>
+      <c r="B236">
+        <v>8</v>
+      </c>
+      <c r="C236">
+        <v>250</v>
+      </c>
+      <c r="D236">
+        <v>100</v>
+      </c>
+      <c r="E236">
+        <v>10</v>
+      </c>
+      <c r="F236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>1</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+      <c r="C237">
+        <v>250</v>
+      </c>
+      <c r="D237">
+        <v>50</v>
+      </c>
+      <c r="E237">
+        <v>8</v>
+      </c>
+      <c r="F237">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>1</v>
+      </c>
+      <c r="B238">
+        <v>3</v>
+      </c>
+      <c r="C238">
+        <v>250</v>
+      </c>
+      <c r="D238">
+        <v>100</v>
+      </c>
+      <c r="E238">
+        <v>10</v>
+      </c>
+      <c r="F238">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>1</v>
+      </c>
+      <c r="B239">
+        <v>6</v>
+      </c>
+      <c r="C239">
+        <v>250</v>
+      </c>
+      <c r="D239">
+        <v>50</v>
+      </c>
+      <c r="E239">
+        <v>9</v>
+      </c>
+      <c r="F239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>1</v>
+      </c>
+      <c r="B240">
+        <v>7</v>
+      </c>
+      <c r="C240">
+        <v>250</v>
+      </c>
+      <c r="D240">
+        <v>100</v>
+      </c>
+      <c r="E240">
+        <v>10</v>
+      </c>
+      <c r="F240">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>1</v>
+      </c>
+      <c r="B241">
+        <v>12</v>
+      </c>
+      <c r="C241">
+        <v>250</v>
+      </c>
+      <c r="D241">
+        <v>50</v>
+      </c>
+      <c r="E241">
+        <v>9</v>
+      </c>
+      <c r="F241">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>1</v>
+      </c>
+      <c r="B242">
+        <v>0</v>
+      </c>
+      <c r="C242">
+        <v>250</v>
+      </c>
+      <c r="D242">
+        <v>50</v>
+      </c>
+      <c r="E242">
+        <v>9</v>
+      </c>
+      <c r="F242">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>1</v>
+      </c>
+      <c r="B243">
+        <v>4</v>
+      </c>
+      <c r="C243">
+        <v>250</v>
+      </c>
+      <c r="D243">
+        <v>50</v>
+      </c>
+      <c r="E243">
+        <v>8</v>
+      </c>
+      <c r="F243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>1</v>
+      </c>
+      <c r="B244">
+        <v>2</v>
+      </c>
+      <c r="C244">
+        <v>250</v>
+      </c>
+      <c r="D244">
+        <v>100</v>
+      </c>
+      <c r="E244">
+        <v>10</v>
+      </c>
+      <c r="F244">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>1</v>
+      </c>
+      <c r="B245">
+        <v>3</v>
+      </c>
+      <c r="C245">
+        <v>250</v>
+      </c>
+      <c r="D245">
+        <v>50</v>
+      </c>
+      <c r="E245">
+        <v>8</v>
+      </c>
+      <c r="F245">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>1</v>
+      </c>
+      <c r="B246">
+        <v>1</v>
+      </c>
+      <c r="C246">
+        <v>250</v>
+      </c>
+      <c r="D246">
+        <v>50</v>
+      </c>
+      <c r="E246">
+        <v>8</v>
+      </c>
+      <c r="F246">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>1</v>
+      </c>
+      <c r="B247">
+        <v>0</v>
+      </c>
+      <c r="C247">
+        <v>275</v>
+      </c>
+      <c r="D247">
+        <v>10</v>
+      </c>
+      <c r="E247">
+        <v>5</v>
+      </c>
+      <c r="F247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>1</v>
+      </c>
+      <c r="B248">
+        <v>0</v>
+      </c>
+      <c r="C248">
+        <v>275</v>
+      </c>
+      <c r="D248">
+        <v>10</v>
+      </c>
+      <c r="E248">
+        <v>5</v>
+      </c>
+      <c r="F248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>1</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="C249">
+        <v>275</v>
+      </c>
+      <c r="D249">
+        <v>20</v>
+      </c>
+      <c r="E249">
+        <v>7</v>
+      </c>
+      <c r="F249">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>1</v>
+      </c>
+      <c r="B250">
+        <v>0</v>
+      </c>
+      <c r="C250">
+        <v>275</v>
+      </c>
+      <c r="D250">
+        <v>10</v>
+      </c>
+      <c r="E250">
+        <v>6</v>
+      </c>
+      <c r="F250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>1</v>
+      </c>
+      <c r="B251">
+        <v>0</v>
+      </c>
+      <c r="C251">
+        <v>275</v>
+      </c>
+      <c r="D251">
+        <v>20</v>
+      </c>
+      <c r="E251">
+        <v>7</v>
+      </c>
+      <c r="F251">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>1</v>
+      </c>
+      <c r="B252">
+        <v>2</v>
+      </c>
+      <c r="C252">
+        <v>275</v>
+      </c>
+      <c r="D252">
+        <v>20</v>
+      </c>
+      <c r="E252">
+        <v>7</v>
+      </c>
+      <c r="F252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>1</v>
+      </c>
+      <c r="B253">
+        <v>0</v>
+      </c>
+      <c r="C253">
+        <v>275</v>
+      </c>
+      <c r="D253">
+        <v>10</v>
+      </c>
+      <c r="E253">
+        <v>6</v>
+      </c>
+      <c r="F253">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>1</v>
+      </c>
+      <c r="B254">
+        <v>0</v>
+      </c>
+      <c r="C254">
+        <v>275</v>
+      </c>
+      <c r="D254">
+        <v>10</v>
+      </c>
+      <c r="E254">
+        <v>5</v>
+      </c>
+      <c r="F254">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>1</v>
+      </c>
+      <c r="B255">
+        <v>0</v>
+      </c>
+      <c r="C255">
+        <v>275</v>
+      </c>
+      <c r="D255">
+        <v>10</v>
+      </c>
+      <c r="E255">
+        <v>6</v>
+      </c>
+      <c r="F255">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>1</v>
+      </c>
+      <c r="B256">
+        <v>0</v>
+      </c>
+      <c r="C256">
+        <v>275</v>
+      </c>
+      <c r="D256">
+        <v>10</v>
+      </c>
+      <c r="E256">
+        <v>6</v>
+      </c>
+      <c r="F256">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>1</v>
+      </c>
+      <c r="B257">
+        <v>0</v>
+      </c>
+      <c r="C257">
+        <v>275</v>
+      </c>
+      <c r="D257">
+        <v>10</v>
+      </c>
+      <c r="E257">
+        <v>5</v>
+      </c>
+      <c r="F257">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>1</v>
+      </c>
+      <c r="B258">
+        <v>2</v>
+      </c>
+      <c r="C258">
+        <v>275</v>
+      </c>
+      <c r="D258">
+        <v>20</v>
+      </c>
+      <c r="E258">
+        <v>7</v>
+      </c>
+      <c r="F258">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>1</v>
+      </c>
+      <c r="B259">
+        <v>2</v>
+      </c>
+      <c r="C259">
+        <v>275</v>
+      </c>
+      <c r="D259">
+        <v>50</v>
+      </c>
+      <c r="E259">
+        <v>8</v>
+      </c>
+      <c r="F259">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>1</v>
+      </c>
+      <c r="B260">
+        <v>3</v>
+      </c>
+      <c r="C260">
+        <v>275</v>
+      </c>
+      <c r="D260">
+        <v>50</v>
+      </c>
+      <c r="E260">
+        <v>8</v>
+      </c>
+      <c r="F260">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>1</v>
+      </c>
+      <c r="B261">
+        <v>1</v>
+      </c>
+      <c r="C261">
+        <v>275</v>
+      </c>
+      <c r="D261">
+        <v>50</v>
+      </c>
+      <c r="E261">
+        <v>8</v>
+      </c>
+      <c r="F261">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>1</v>
+      </c>
+      <c r="B262">
+        <v>6</v>
+      </c>
+      <c r="C262">
+        <v>275</v>
+      </c>
+      <c r="D262">
+        <v>50</v>
+      </c>
+      <c r="E262">
+        <v>9</v>
+      </c>
+      <c r="F262">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>1</v>
+      </c>
+      <c r="B263">
+        <v>4</v>
+      </c>
+      <c r="C263">
+        <v>275</v>
+      </c>
+      <c r="D263">
+        <v>50</v>
+      </c>
+      <c r="E263">
+        <v>9</v>
+      </c>
+      <c r="F263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>1</v>
+      </c>
+      <c r="B264">
+        <v>8</v>
+      </c>
+      <c r="C264">
+        <v>275</v>
+      </c>
+      <c r="D264">
+        <v>100</v>
+      </c>
+      <c r="E264">
+        <v>10</v>
+      </c>
+      <c r="F264">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>1</v>
+      </c>
+      <c r="B265">
+        <v>2</v>
+      </c>
+      <c r="C265">
+        <v>275</v>
+      </c>
+      <c r="D265">
+        <v>50</v>
+      </c>
+      <c r="E265">
+        <v>8</v>
+      </c>
+      <c r="F265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>1</v>
+      </c>
+      <c r="B266">
+        <v>7</v>
+      </c>
+      <c r="C266">
+        <v>275</v>
+      </c>
+      <c r="D266">
+        <v>100</v>
+      </c>
+      <c r="E266">
+        <v>10</v>
+      </c>
+      <c r="F266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>1</v>
+      </c>
+      <c r="B267">
+        <v>0</v>
+      </c>
+      <c r="C267">
+        <v>275</v>
+      </c>
+      <c r="D267">
+        <v>50</v>
+      </c>
+      <c r="E267">
+        <v>9</v>
+      </c>
+      <c r="F267">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>1</v>
+      </c>
+      <c r="B268">
+        <v>6</v>
+      </c>
+      <c r="C268">
+        <v>275</v>
+      </c>
+      <c r="D268">
+        <v>100</v>
+      </c>
+      <c r="E268">
+        <v>10</v>
+      </c>
+      <c r="F268">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>1</v>
+      </c>
+      <c r="B269">
+        <v>3</v>
+      </c>
+      <c r="C269">
+        <v>275</v>
+      </c>
+      <c r="D269">
+        <v>100</v>
+      </c>
+      <c r="E269">
+        <v>10</v>
+      </c>
+      <c r="F269">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>1</v>
+      </c>
+      <c r="B270">
+        <v>0</v>
+      </c>
+      <c r="C270">
+        <v>300</v>
+      </c>
+      <c r="D270">
+        <v>20</v>
+      </c>
+      <c r="E270">
+        <v>7</v>
+      </c>
+      <c r="F270">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>1</v>
+      </c>
+      <c r="B271">
+        <v>5</v>
+      </c>
+      <c r="C271">
+        <v>300</v>
+      </c>
+      <c r="D271">
+        <v>20</v>
+      </c>
+      <c r="E271">
+        <v>7</v>
+      </c>
+      <c r="F271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>1</v>
+      </c>
+      <c r="B272">
+        <v>3</v>
+      </c>
+      <c r="C272">
+        <v>300</v>
+      </c>
+      <c r="D272">
+        <v>20</v>
+      </c>
+      <c r="E272">
+        <v>7</v>
+      </c>
+      <c r="F272">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>1</v>
+      </c>
+      <c r="B273">
+        <v>0</v>
+      </c>
+      <c r="C273">
+        <v>300</v>
+      </c>
+      <c r="D273">
+        <v>10</v>
+      </c>
+      <c r="E273">
+        <v>6</v>
+      </c>
+      <c r="F273">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>1</v>
+      </c>
+      <c r="B274">
+        <v>0</v>
+      </c>
+      <c r="C274">
+        <v>300</v>
+      </c>
+      <c r="D274">
+        <v>10</v>
+      </c>
+      <c r="E274">
+        <v>6</v>
+      </c>
+      <c r="F274">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>1</v>
+      </c>
+      <c r="B275">
+        <v>1</v>
+      </c>
+      <c r="C275">
+        <v>300</v>
+      </c>
+      <c r="D275">
+        <v>20</v>
+      </c>
+      <c r="E275">
+        <v>7</v>
+      </c>
+      <c r="F275">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>1</v>
+      </c>
+      <c r="B276">
+        <v>0</v>
+      </c>
+      <c r="C276">
+        <v>300</v>
+      </c>
+      <c r="D276">
+        <v>10</v>
+      </c>
+      <c r="E276">
+        <v>6</v>
+      </c>
+      <c r="F276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>1</v>
+      </c>
+      <c r="B277">
+        <v>0</v>
+      </c>
+      <c r="C277">
+        <v>300</v>
+      </c>
+      <c r="D277">
+        <v>10</v>
+      </c>
+      <c r="E277">
+        <v>5</v>
+      </c>
+      <c r="F277">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>1</v>
+      </c>
+      <c r="B278">
+        <v>0</v>
+      </c>
+      <c r="C278">
+        <v>300</v>
+      </c>
+      <c r="D278">
+        <v>10</v>
+      </c>
+      <c r="E278">
+        <v>6</v>
+      </c>
+      <c r="F278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>1</v>
+      </c>
+      <c r="B279">
+        <v>0</v>
+      </c>
+      <c r="C279">
+        <v>300</v>
+      </c>
+      <c r="D279">
+        <v>10</v>
+      </c>
+      <c r="E279">
+        <v>5</v>
+      </c>
+      <c r="F279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>1</v>
+      </c>
+      <c r="B280">
+        <v>0</v>
+      </c>
+      <c r="C280">
+        <v>300</v>
+      </c>
+      <c r="D280">
+        <v>10</v>
+      </c>
+      <c r="E280">
+        <v>5</v>
+      </c>
+      <c r="F280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>1</v>
+      </c>
+      <c r="B281">
+        <v>0</v>
+      </c>
+      <c r="C281">
+        <v>300</v>
+      </c>
+      <c r="D281">
+        <v>10</v>
+      </c>
+      <c r="E281">
+        <v>5</v>
+      </c>
+      <c r="F281">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>1</v>
+      </c>
+      <c r="B282">
+        <v>6</v>
+      </c>
+      <c r="C282">
+        <v>300</v>
+      </c>
+      <c r="D282">
+        <v>100</v>
+      </c>
+      <c r="E282">
+        <v>10</v>
+      </c>
+      <c r="F282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>1</v>
+      </c>
+      <c r="B283">
+        <v>3</v>
+      </c>
+      <c r="C283">
+        <v>300</v>
+      </c>
+      <c r="D283">
+        <v>50</v>
+      </c>
+      <c r="E283">
+        <v>8</v>
+      </c>
+      <c r="F283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>1</v>
+      </c>
+      <c r="B284">
+        <v>6</v>
+      </c>
+      <c r="C284">
+        <v>300</v>
+      </c>
+      <c r="D284">
+        <v>100</v>
+      </c>
+      <c r="E284">
+        <v>10</v>
+      </c>
+      <c r="F284">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>1</v>
+      </c>
+      <c r="B285">
+        <v>10</v>
+      </c>
+      <c r="C285">
+        <v>300</v>
+      </c>
+      <c r="D285">
+        <v>100</v>
+      </c>
+      <c r="E285">
+        <v>10</v>
+      </c>
+      <c r="F285">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>1</v>
+      </c>
+      <c r="B286">
+        <v>6</v>
+      </c>
+      <c r="C286">
+        <v>300</v>
+      </c>
+      <c r="D286">
+        <v>50</v>
+      </c>
+      <c r="E286">
+        <v>9</v>
+      </c>
+      <c r="F286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>1</v>
+      </c>
+      <c r="B287">
+        <v>1</v>
+      </c>
+      <c r="C287">
+        <v>300</v>
+      </c>
+      <c r="D287">
+        <v>50</v>
+      </c>
+      <c r="E287">
+        <v>8</v>
+      </c>
+      <c r="F287">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>1</v>
+      </c>
+      <c r="B288">
+        <v>2</v>
+      </c>
+      <c r="C288">
+        <v>300</v>
+      </c>
+      <c r="D288">
+        <v>100</v>
+      </c>
+      <c r="E288">
+        <v>10</v>
+      </c>
+      <c r="F288">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>1</v>
+      </c>
+      <c r="B289">
+        <v>2</v>
+      </c>
+      <c r="C289">
+        <v>300</v>
+      </c>
+      <c r="D289">
+        <v>50</v>
+      </c>
+      <c r="E289">
+        <v>8</v>
+      </c>
+      <c r="F289">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>1</v>
+      </c>
+      <c r="B290">
+        <v>0</v>
+      </c>
+      <c r="C290">
+        <v>300</v>
+      </c>
+      <c r="D290">
+        <v>50</v>
+      </c>
+      <c r="E290">
+        <v>9</v>
+      </c>
+      <c r="F290">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>1</v>
+      </c>
+      <c r="B291">
+        <v>2</v>
+      </c>
+      <c r="C291">
+        <v>300</v>
+      </c>
+      <c r="D291">
+        <v>50</v>
+      </c>
+      <c r="E291">
+        <v>8</v>
+      </c>
+      <c r="F291">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amount of plateau updates
</commit_message>
<xml_diff>
--- a/Models to measure/Results/Filtered loss plots/Amount of plateaus.xlsx
+++ b/Models to measure/Results/Filtered loss plots/Amount of plateaus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20182672\Documents\GitHub\Final_Project\Models to measure\Results\Filtered loss plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DCBB41-ED45-4E4D-87E9-8D12C038977B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BDEB9B-85A8-4D93-A269-E184F5494BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98A813E1-F41E-4DF4-9B2F-04D1C5B250A2}"/>
+    <workbookView xWindow="2490" yWindow="1845" windowWidth="21600" windowHeight="11325" xr2:uid="{98A813E1-F41E-4DF4-9B2F-04D1C5B250A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED336A5-05FC-4E6D-9199-11645426FC6F}">
   <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
-      <selection activeCell="F293" sqref="F293"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="H150" sqref="H150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>